<commit_message>
chore!: new input variable in sheet CONDUCTOR_operation of file conductor_definition
New flag SELF_INDUCTANCE_MODE allows user to select how to evaluate the self iductances. Valid only if flag INDUCTANCE_MODE is set to 1 (analytical).
</commit_message>
<xml_diff>
--- a/source_code/input_files/input_file_template/template_conductor_definition.xlsx
+++ b/source_code/input_files/input_file_template/template_conductor_definition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://politoit-my.sharepoint.com/personal/daniele_placido_polito_it/Documents/OPENSC2/source_code/input_files/input_file_template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="69" documentId="13_ncr:1_{A4BE69DD-9F2A-474B-96DB-7E8A1B3E00C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E0CA9FE2-2263-49B5-B3B9-B3A526246EEA}"/>
+  <xr:revisionPtr revIDLastSave="81" documentId="13_ncr:1_{A4BE69DD-9F2A-474B-96DB-7E8A1B3E00C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{75E81E8A-3CD6-4807-B0AB-FEB266191791}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CONDUCTOR_files" sheetId="6" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="85">
   <si>
     <t>m</t>
   </si>
@@ -257,9 +257,6 @@
     <t>INDUCTANCE_MODE</t>
   </si>
   <si>
-    <t>flag to select the method to evaluate the inductance. Possible values: 0 = iterative; 1 = analytical. Defaults to 0</t>
-  </si>
-  <si>
     <t>I0_OP_MODE</t>
   </si>
   <si>
@@ -288,6 +285,15 @@
   </si>
   <si>
     <t>Length of the conductor along the z axis</t>
+  </si>
+  <si>
+    <t>SELF_INDUCTANCE_MODE</t>
+  </si>
+  <si>
+    <t>flag to select the method to evaluate the self inductance. Possible values: 1 = mode 1; 2 = mode 2. Used only if flag INDUCTANCE_MODE is set to 1. Defaults to 2</t>
+  </si>
+  <si>
+    <t>flag to select the method to evaluate the inductance. Possible values: 0 = analytical; 1 = approximated. Defaults to 1.</t>
   </si>
 </sst>
 </file>
@@ -1074,7 +1080,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C2D1443-3A2D-4AC0-948E-E6BCBD41CD63}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
@@ -1135,7 +1141,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>0</v>
@@ -1144,7 +1150,7 @@
         <v>16</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E4" s="4">
         <v>10</v>
@@ -1220,7 +1226,7 @@
     </row>
     <row r="9" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>3</v>
@@ -1229,7 +1235,7 @@
         <v>17</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E9" s="5">
         <v>0</v>
@@ -1237,7 +1243,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>2</v>
@@ -1442,7 +1448,7 @@
     </row>
     <row r="22" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="34" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B22" s="35" t="s">
         <v>15</v>
@@ -1451,7 +1457,7 @@
         <v>18</v>
       </c>
       <c r="D22" s="38" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E22" s="35" t="s">
         <v>35</v>
@@ -1459,7 +1465,7 @@
     </row>
     <row r="23" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A23" s="34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B23" s="35" t="s">
         <v>4</v>
@@ -1468,10 +1474,10 @@
         <v>16</v>
       </c>
       <c r="D23" s="38" t="s">
+        <v>78</v>
+      </c>
+      <c r="E23" s="35" t="s">
         <v>79</v>
-      </c>
-      <c r="E23" s="35" t="s">
-        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1483,10 +1489,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC5BD13E-E4E6-4E9C-8F28-77E32E58E378}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:O1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1619,10 +1625,27 @@
         <v>17</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="E8" s="33">
-        <v>0</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="E9" s="33">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat!: new input variable in sheet CONDUCTOR_operation of file conductor_definition
Variable ELECTRIC_SOLVER allows user to specifiy if the electric problem should be solved appliyng steady state or transient solution tecniques.
</commit_message>
<xml_diff>
--- a/source_code/input_files/input_file_template/template_conductor_definition.xlsx
+++ b/source_code/input_files/input_file_template/template_conductor_definition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://politoit-my.sharepoint.com/personal/daniele_placido_polito_it/Documents/OPENSC2/source_code/input_files/input_file_template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="81" documentId="13_ncr:1_{A4BE69DD-9F2A-474B-96DB-7E8A1B3E00C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{75E81E8A-3CD6-4807-B0AB-FEB266191791}"/>
+  <xr:revisionPtr revIDLastSave="90" documentId="13_ncr:1_{A4BE69DD-9F2A-474B-96DB-7E8A1B3E00C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B5B20D1-8587-49EE-8B6A-D93A7C8E7DC5}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="87">
   <si>
     <t>m</t>
   </si>
@@ -294,6 +294,12 @@
   </si>
   <si>
     <t>flag to select the method to evaluate the inductance. Possible values: 0 = analytical; 1 = approximated. Defaults to 1.</t>
+  </si>
+  <si>
+    <t>ELECTRIC_SOLVER</t>
+  </si>
+  <si>
+    <t>Flag to select the solver for the electric module. Possible values: 0= steady state; 1 = transient. Defaults to 1</t>
   </si>
 </sst>
 </file>
@@ -1489,10 +1495,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC5BD13E-E4E6-4E9C-8F28-77E32E58E378}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1646,6 +1652,23 @@
       </c>
       <c r="E9" s="33">
         <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="E10" s="33">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: update note in sheet CONDUCTOR_operation
Updated note for variable ELECTRIC_SOLVER.
</commit_message>
<xml_diff>
--- a/source_code/input_files/input_file_template/template_conductor_definition.xlsx
+++ b/source_code/input_files/input_file_template/template_conductor_definition.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://politoit-my.sharepoint.com/personal/daniele_placido_polito_it/Documents/OPENSC2/source_code/input_files/input_file_template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniele.placido\3D Objects\OPENSC2\source_code\input_files\input_file_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="92" documentId="13_ncr:1_{A4BE69DD-9F2A-474B-96DB-7E8A1B3E00C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{869E9A8C-4085-492C-8B2C-7ADC41E31303}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7B09D77-AF54-42D7-A30D-A705D7436731}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1860" yWindow="1860" windowWidth="21600" windowHeight="11295" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CONDUCTOR_files" sheetId="6" r:id="rId1"/>
@@ -296,10 +296,10 @@
     <t>ELECTRIC_SOLVER</t>
   </si>
   <si>
-    <t>Flag to select the solver for the electric module. Possible values: 0= steady state; 1 = transient. Defaults to 1</t>
-  </si>
-  <si>
-    <t>time step value for the electric transient solution. If None, uses the default value of dt_th/500, being dt_th the thermal time step.</t>
+    <t>time step value for the electric transient solution. If None, uses the default value of dt_th/10, being dt_th the thermal time step.</t>
+  </si>
+  <si>
+    <t>Flag to select the solver for the electric module. Possible values: 0= steady state; 1 = transient. Defaults to 1. N.B. At the time being the steady solution is not availabye, althoug it works, to be consistent with the thermal hydrauilc solution.</t>
   </si>
 </sst>
 </file>
@@ -355,28 +355,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -387,85 +368,50 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -837,65 +783,66 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C37" sqref="C37"/>
+      <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.453125" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.453125" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.81640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.54296875" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.81640625" style="7"/>
+    <col min="1" max="1" width="20.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="9">
+      <c r="B1" s="7">
         <f>SUM(E2:AE2)</f>
         <v>1</v>
       </c>
-      <c r="D1" s="3"/>
+      <c r="C1" s="2"/>
       <c r="E1" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="12"/>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="10"/>
+      <c r="B2" s="2"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="9">
+      <c r="D2" s="15"/>
+      <c r="E2" s="7">
         <f>IF(E$1 &gt; 0,1,0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="11" t="str">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="str">
         <f>[1]TRANSIENT!A$2</f>
         <v>Variable name</v>
       </c>
-      <c r="B3" s="11" t="str">
+      <c r="B3" s="9" t="str">
         <f>[1]TRANSIENT!B$2</f>
         <v>Unit</v>
       </c>
-      <c r="C3" s="11" t="str">
+      <c r="C3" s="9" t="str">
         <f>[1]TRANSIENT!C$2</f>
         <v>Variable type</v>
       </c>
-      <c r="D3" s="11" t="str">
+      <c r="D3" s="9" t="str">
         <f>[1]TRANSIENT!D$2</f>
         <v>Note/comments</v>
       </c>
-      <c r="E3" s="9" t="str">
+      <c r="E3" s="7" t="str">
         <f>_xlfn.TEXTJOIN("_",,$A$1,E$1)</f>
         <v>CONDUCTOR_1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="15" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -904,12 +851,13 @@
       <c r="C4" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="D4" s="2"/>
       <c r="E4" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="15" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -918,13 +866,13 @@
       <c r="C5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="14"/>
+      <c r="D5" s="12"/>
       <c r="E5" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="15" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -933,13 +881,13 @@
       <c r="C6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="14"/>
+      <c r="D6" s="12"/>
       <c r="E6" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="15" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -948,14 +896,14 @@
       <c r="C7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="14"/>
+      <c r="D7" s="12"/>
       <c r="E7" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="15" t="s">
-        <v>13</v>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>15</v>
@@ -963,14 +911,14 @@
       <c r="C8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="14"/>
+      <c r="D8" s="11"/>
       <c r="E8" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="15" t="s">
-        <v>11</v>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>13</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>15</v>
@@ -978,14 +926,14 @@
       <c r="C9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="13"/>
+      <c r="D9" s="12"/>
       <c r="E9" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="15" t="s">
-        <v>23</v>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>15</v>
@@ -993,14 +941,14 @@
       <c r="C10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="13"/>
+      <c r="D10" s="11"/>
       <c r="E10" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="15" t="s">
-        <v>20</v>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>23</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>15</v>
@@ -1008,14 +956,14 @@
       <c r="C11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="13"/>
+      <c r="D11" s="11"/>
       <c r="E11" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="15" t="s">
-        <v>12</v>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>20</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>15</v>
@@ -1023,14 +971,14 @@
       <c r="C12" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="13"/>
+      <c r="D12" s="11"/>
       <c r="E12" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="15" t="s">
-        <v>14</v>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>15</v>
@@ -1038,40 +986,40 @@
       <c r="C13" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="13"/>
+      <c r="D13" s="11"/>
       <c r="E13" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="23" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="21" t="s">
+    <row r="14" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="22"/>
-      <c r="E14" s="21" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="24" t="s">
+      <c r="D14" s="11"/>
+      <c r="E14" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="21" t="s">
+      <c r="B15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="25" t="s">
+      <c r="D15" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E15" s="25" t="s">
+      <c r="E15" s="3" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1086,67 +1034,67 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C2D1443-3A2D-4AC0-948E-E6BCBD41CD63}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.54296875" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.453125" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.81640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.453125" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7265625" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="7"/>
+    <col min="1" max="1" width="19.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="str">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="str">
         <f>CONDUCTOR_files!A$1</f>
         <v>CONDUCTOR</v>
       </c>
-      <c r="B1" s="18">
+      <c r="B1" s="14">
         <f>SUM(E2:AE2)</f>
         <v>1</v>
       </c>
-      <c r="E1" s="18">
+      <c r="E1" s="14">
         <f>CONDUCTOR_files!E$1</f>
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E2" s="18">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E2" s="14">
         <f>IF(E$1 &gt; 0,1,0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="16" t="str">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="str">
         <f>CONDUCTOR_files!A$3</f>
         <v>Variable name</v>
       </c>
-      <c r="B3" s="16" t="str">
+      <c r="B3" s="13" t="str">
         <f>CONDUCTOR_files!B$3</f>
         <v>Unit</v>
       </c>
-      <c r="C3" s="16" t="str">
+      <c r="C3" s="13" t="str">
         <f>CONDUCTOR_files!C$3</f>
         <v>Variable type</v>
       </c>
-      <c r="D3" s="16" t="str">
+      <c r="D3" s="13" t="str">
         <f>CONDUCTOR_files!D$3</f>
         <v>Note/comments</v>
       </c>
-      <c r="E3" s="18" t="str">
+      <c r="E3" s="14" t="str">
         <f>_xlfn.TEXTJOIN("_",,$A$1,E$1)</f>
         <v>CONDUCTOR_1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="15" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
         <v>79</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -1155,15 +1103,15 @@
       <c r="C4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="12" t="s">
         <v>80</v>
       </c>
       <c r="E4" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="15" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>47</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -1172,15 +1120,15 @@
       <c r="C5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="12" t="s">
         <v>48</v>
       </c>
       <c r="E5" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="15" t="s">
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
         <v>49</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -1189,15 +1137,15 @@
       <c r="C6" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="12" t="s">
         <v>51</v>
       </c>
       <c r="E6" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="15" t="s">
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
         <v>52</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -1206,15 +1154,15 @@
       <c r="C7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="12" t="s">
         <v>54</v>
       </c>
       <c r="E7" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="15" t="s">
+    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
         <v>53</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -1223,15 +1171,15 @@
       <c r="C8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="12" t="s">
         <v>55</v>
       </c>
       <c r="E8" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="15" t="s">
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
         <v>72</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -1240,15 +1188,15 @@
       <c r="C9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="12" t="s">
         <v>74</v>
       </c>
       <c r="E9" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="15" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
         <v>73</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -1257,15 +1205,15 @@
       <c r="C10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="12" t="s">
         <v>24</v>
       </c>
       <c r="E10" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="15" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -1274,15 +1222,15 @@
       <c r="C11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="12" t="s">
         <v>25</v>
       </c>
       <c r="E11" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="15" t="s">
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
         <v>21</v>
       </c>
       <c r="B12" s="6" t="s">
@@ -1291,15 +1239,15 @@
       <c r="C12" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="12" t="s">
         <v>26</v>
       </c>
       <c r="E12" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="15" t="s">
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -1308,15 +1256,15 @@
       <c r="C13" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="12" t="s">
         <v>27</v>
       </c>
       <c r="E13" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="15" t="s">
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -1325,15 +1273,15 @@
       <c r="C14" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="12" t="s">
         <v>28</v>
       </c>
       <c r="E14" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="15" t="s">
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -1342,147 +1290,147 @@
       <c r="C15" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="D15" s="12" t="s">
         <v>29</v>
       </c>
       <c r="E15" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16" s="10" t="s">
+    <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="17" t="s">
+      <c r="D16" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="E16" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A17" s="10" t="s">
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="17" t="s">
+      <c r="D17" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E17" s="8">
+      <c r="E17" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="10" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="8" t="s">
+      <c r="B18" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E18" s="10" t="str">
+      <c r="E18" s="8" t="str">
         <f>E$3</f>
         <v>CONDUCTOR_1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="17" t="s">
+    <row r="19" spans="1:5" ht="225" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" s="8" t="s">
+      <c r="B19" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="17" t="s">
+      <c r="D19" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="E19" s="17" t="s">
+      <c r="E19" s="12" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="10" t="s">
+    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" s="8" t="s">
+      <c r="B20" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D20" s="27" t="s">
+      <c r="D20" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="E20" s="8">
+      <c r="E20" s="3">
         <v>0.5</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="10" t="s">
+    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" s="8" t="s">
+      <c r="B21" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="27" t="s">
+      <c r="D21" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="E21" s="8">
+      <c r="E21" s="3">
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A22" s="34" t="s">
+    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="B22" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" s="35" t="s">
+      <c r="B22" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D22" s="38" t="s">
+      <c r="D22" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="E22" s="35" t="s">
+      <c r="E22" s="19" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="34" t="s">
+    <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="B23" s="35" t="s">
+      <c r="B23" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="C23" s="35" t="s">
+      <c r="C23" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D23" s="38" t="s">
-        <v>86</v>
-      </c>
-      <c r="E23" s="35" t="s">
+      <c r="D23" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="E23" s="19" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1497,177 +1445,177 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC5BD13E-E4E6-4E9C-8F28-77E32E58E378}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="31" t="str">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="str">
         <f>CONDUCTOR_files!A1</f>
         <v>CONDUCTOR</v>
       </c>
-      <c r="B1" s="31">
+      <c r="B1" s="13">
         <f>SUM(E2:U2)</f>
         <v>1</v>
       </c>
-      <c r="E1" s="32">
+      <c r="E1" s="14">
         <f>CONDUCTOR_files!E1</f>
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E2" s="32">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E2" s="14">
         <f>IF(E$1 &gt;0,1,0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="31" t="str">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="str">
         <f>CONDUCTOR_files!A$3</f>
         <v>Variable name</v>
       </c>
-      <c r="B3" s="31" t="str">
+      <c r="B3" s="13" t="str">
         <f>CONDUCTOR_files!B$3</f>
         <v>Unit</v>
       </c>
-      <c r="C3" s="31" t="str">
+      <c r="C3" s="13" t="str">
         <f>CONDUCTOR_files!C$3</f>
         <v>Variable type</v>
       </c>
-      <c r="D3" s="31" t="str">
+      <c r="D3" s="13" t="str">
         <f>CONDUCTOR_files!D$3</f>
         <v>Note/comments</v>
       </c>
-      <c r="E3" s="31" t="str">
+      <c r="E3" s="13" t="str">
         <f>CONDUCTOR_files!E3</f>
         <v>CONDUCTOR_1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="174" x14ac:dyDescent="0.35">
-      <c r="A4" s="34" t="s">
+    <row r="4" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="8" t="s">
+      <c r="B4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="E4" s="29" t="b">
+      <c r="E4" s="4" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="87" x14ac:dyDescent="0.35">
-      <c r="A5" s="34" t="s">
+    <row r="5" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="8" t="s">
+      <c r="B5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="D5" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="E5" s="30">
+      <c r="E5" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="34" t="s">
+    <row r="6" spans="1:5" ht="210" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="8" t="s">
+      <c r="B6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="27" t="s">
+      <c r="D6" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="E6" s="29" t="s">
+      <c r="E6" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="87" x14ac:dyDescent="0.35">
-      <c r="A7" s="34" t="s">
+    <row r="7" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="B7" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="35" t="s">
+      <c r="B7" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="36" t="s">
+      <c r="D7" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="E7" s="37">
+      <c r="E7" s="21">
         <v>1000</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="116" x14ac:dyDescent="0.35">
-      <c r="A8" s="34" t="s">
+    <row r="8" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A8" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="8" t="s">
+      <c r="B8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="27" t="s">
+      <c r="D8" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="E8" s="33">
+      <c r="E8" s="17">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="34" t="s">
+    <row r="9" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="B9" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="8" t="s">
+      <c r="B9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="27" t="s">
+      <c r="D9" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="E9" s="33">
+      <c r="E9" s="17">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="34" t="s">
+    <row r="10" spans="1:5" ht="270" x14ac:dyDescent="0.25">
+      <c r="A10" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="B10" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="8" t="s">
+      <c r="B10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="27" t="s">
-        <v>85</v>
-      </c>
-      <c r="E10" s="33">
+      <c r="D10" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="E10" s="17">
         <v>1</v>
       </c>
     </row>
@@ -1684,25 +1632,24 @@
       <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="13.54296875" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="28"/>
-      <c r="B1" s="28" t="str">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" t="str">
         <f>CONDUCTOR_files!E$3</f>
         <v>CONDUCTOR_1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="28" t="str">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="str">
         <f>B1</f>
         <v>CONDUCTOR_1</v>
       </c>
-      <c r="B2" s="28">
+      <c r="B2">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
chore: update note/commit in input file
Added an explatation to the value none for flag I0_OP_MODE in sheet CONDUCTOR_input in the input file template_conductor_definition.xlsx.
</commit_message>
<xml_diff>
--- a/source_code/input_files/input_file_template/template_conductor_definition.xlsx
+++ b/source_code/input_files/input_file_template/template_conductor_definition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniele.placido\3D Objects\OPENSC2\source_code\input_files\input_file_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7B09D77-AF54-42D7-A30D-A705D7436731}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{822FE799-45CB-4BB4-AEC1-82C5AC2B334C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="1860" windowWidth="21600" windowHeight="11295" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CONDUCTOR_files" sheetId="6" r:id="rId1"/>
@@ -263,9 +263,6 @@
     <t>I0_OP_TOT</t>
   </si>
   <si>
-    <t>current flag: 0 = constant; -1 = read from file; -2 = external function for current and its derivative after taudum</t>
-  </si>
-  <si>
     <t>ELECTRIC_METHOD</t>
   </si>
   <si>
@@ -300,6 +297,9 @@
   </si>
   <si>
     <t>Flag to select the solver for the electric module. Possible values: 0= steady state; 1 = transient. Defaults to 1. N.B. At the time being the steady solution is not availabye, althoug it works, to be consistent with the thermal hydrauilc solution.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">current flag: none = current is not defined, bypass the electric module; 0 = constant; -1 = read from file; -2 = external function for current and its derivative after taudum; </t>
   </si>
 </sst>
 </file>
@@ -1034,11 +1034,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C2D1443-3A2D-4AC0-948E-E6BCBD41CD63}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D24" sqref="D24"/>
+      <selection pane="bottomRight" activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1095,7 +1095,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>0</v>
@@ -1104,7 +1104,7 @@
         <v>16</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E4" s="4">
         <v>10</v>
@@ -1178,7 +1178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>72</v>
       </c>
@@ -1189,7 +1189,7 @@
         <v>17</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="E9" s="5">
         <v>0</v>
@@ -1402,7 +1402,7 @@
     </row>
     <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B22" s="19" t="s">
         <v>15</v>
@@ -1411,7 +1411,7 @@
         <v>18</v>
       </c>
       <c r="D22" s="22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E22" s="19" t="s">
         <v>35</v>
@@ -1419,7 +1419,7 @@
     </row>
     <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B23" s="19" t="s">
         <v>4</v>
@@ -1428,10 +1428,10 @@
         <v>16</v>
       </c>
       <c r="D23" s="22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E23" s="19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1445,7 +1445,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC5BD13E-E4E6-4E9C-8F28-77E32E58E378}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -1579,7 +1579,7 @@
         <v>17</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E8" s="17">
         <v>1</v>
@@ -1587,7 +1587,7 @@
     </row>
     <row r="9" spans="1:5" ht="165" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>15</v>
@@ -1596,7 +1596,7 @@
         <v>17</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E9" s="17">
         <v>2</v>
@@ -1604,7 +1604,7 @@
     </row>
     <row r="10" spans="1:5" ht="270" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>15</v>
@@ -1613,7 +1613,7 @@
         <v>17</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E10" s="17">
         <v>1</v>

</xml_diff>

<commit_message>
chore!: new variable in sheet CONDUCTOR_file of conductor_definition.xlsx
BREAKING CHANGES: added new variable VARIABLE_CONTACT_PERIMETER in sheet CONDUCTOR_file of input file conductor_definition.xlsx. This variable stores the name of the user defined auxiliary input file (e.g.,variable_contact_perimeter.xlsx) to be used to assign a variable contact perimeter between conductor components.

modified:   input_files/input_file_template/template_conductor_definition.xlsx
</commit_message>
<xml_diff>
--- a/source_code/input_files/input_file_template/template_conductor_definition.xlsx
+++ b/source_code/input_files/input_file_template/template_conductor_definition.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniele.placido\3D Objects\OPENSC2\source_code\input_files\input_file_template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniele.Placido\3D Objects\OPENSC2\source_code\input_files\input_file_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{822FE799-45CB-4BB4-AEC1-82C5AC2B334C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D942AE4-CC28-4E5D-A4BC-B8EB27D3B041}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CONDUCTOR_files" sheetId="6" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="89">
   <si>
     <t>m</t>
   </si>
@@ -300,6 +300,12 @@
   </si>
   <si>
     <t xml:space="preserve">current flag: none = current is not defined, bypass the electric module; 0 = constant; -1 = read from file; -2 = external function for current and its derivative after taudum; </t>
+  </si>
+  <si>
+    <t>VARIABLE_CONTACT_PERIMETER</t>
+  </si>
+  <si>
+    <t>external file for variable contact perimeter. Valid extension .xlsx</t>
   </si>
 </sst>
 </file>
@@ -453,7 +459,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="TRANSIENT"/>
@@ -777,26 +783,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
+      <selection pane="bottomRight" activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.453125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.453125" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.54296875" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="33" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="2"/>
+    <col min="6" max="16384" width="8.81640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>1</v>
       </c>
@@ -809,7 +815,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="10"/>
       <c r="B2" s="2"/>
       <c r="C2" s="1"/>
@@ -819,7 +825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="str">
         <f>[1]TRANSIENT!A$2</f>
         <v>Variable name</v>
@@ -841,7 +847,7 @@
         <v>CONDUCTOR_1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
@@ -856,7 +862,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>6</v>
       </c>
@@ -871,7 +877,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>7</v>
       </c>
@@ -886,7 +892,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
         <v>19</v>
       </c>
@@ -901,7 +907,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
         <v>30</v>
       </c>
@@ -916,7 +922,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
         <v>13</v>
       </c>
@@ -931,7 +937,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
         <v>11</v>
       </c>
@@ -946,7 +952,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
         <v>23</v>
       </c>
@@ -961,7 +967,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
         <v>20</v>
       </c>
@@ -976,7 +982,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
         <v>12</v>
       </c>
@@ -991,7 +997,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
         <v>14</v>
       </c>
@@ -1006,7 +1012,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="8" t="s">
         <v>38</v>
       </c>
@@ -1020,6 +1026,23 @@
         <v>39</v>
       </c>
       <c r="E15" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1034,24 +1057,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C2D1443-3A2D-4AC0-948E-E6BCBD41CD63}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.7109375" style="2"/>
+    <col min="1" max="1" width="19.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="str">
         <f>CONDUCTOR_files!A$1</f>
         <v>CONDUCTOR</v>
@@ -1065,13 +1088,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="E2" s="14">
         <f>IF(E$1 &gt; 0,1,0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="str">
         <f>CONDUCTOR_files!A$3</f>
         <v>Variable name</v>
@@ -1093,7 +1116,7 @@
         <v>CONDUCTOR_1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
         <v>78</v>
       </c>
@@ -1110,7 +1133,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>47</v>
       </c>
@@ -1127,7 +1150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>49</v>
       </c>
@@ -1144,7 +1167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
         <v>52</v>
       </c>
@@ -1161,7 +1184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
         <v>53</v>
       </c>
@@ -1178,7 +1201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
         <v>72</v>
       </c>
@@ -1195,7 +1218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
         <v>73</v>
       </c>
@@ -1212,7 +1235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
         <v>10</v>
       </c>
@@ -1229,7 +1252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
         <v>21</v>
       </c>
@@ -1246,7 +1269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
         <v>22</v>
       </c>
@@ -1263,7 +1286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
         <v>9</v>
       </c>
@@ -1280,7 +1303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="8" t="s">
         <v>8</v>
       </c>
@@ -1297,7 +1320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="8" t="s">
         <v>33</v>
       </c>
@@ -1314,7 +1337,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="8" t="s">
         <v>32</v>
       </c>
@@ -1331,7 +1354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="8" t="s">
         <v>36</v>
       </c>
@@ -1349,7 +1372,7 @@
         <v>CONDUCTOR_1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="225" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A19" s="12" t="s">
         <v>40</v>
       </c>
@@ -1366,7 +1389,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A20" s="8" t="s">
         <v>43</v>
       </c>
@@ -1383,7 +1406,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A21" s="8" t="s">
         <v>44</v>
       </c>
@@ -1400,7 +1423,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="18" t="s">
         <v>74</v>
       </c>
@@ -1417,7 +1440,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A23" s="18" t="s">
         <v>76</v>
       </c>
@@ -1449,16 +1472,16 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="str">
         <f>CONDUCTOR_files!A1</f>
         <v>CONDUCTOR</v>
@@ -1472,13 +1495,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="E2" s="14">
         <f>IF(E$1 &gt;0,1,0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="str">
         <f>CONDUCTOR_files!A$3</f>
         <v>Variable name</v>
@@ -1500,7 +1523,7 @@
         <v>CONDUCTOR_1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="174" x14ac:dyDescent="0.35">
       <c r="A4" s="18" t="s">
         <v>62</v>
       </c>
@@ -1517,7 +1540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A5" s="18" t="s">
         <v>64</v>
       </c>
@@ -1534,7 +1557,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="210" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A6" s="18" t="s">
         <v>66</v>
       </c>
@@ -1551,7 +1574,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A7" s="18" t="s">
         <v>69</v>
       </c>
@@ -1568,7 +1591,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="116" x14ac:dyDescent="0.35">
       <c r="A8" s="18" t="s">
         <v>71</v>
       </c>
@@ -1585,7 +1608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A9" s="18" t="s">
         <v>80</v>
       </c>
@@ -1602,7 +1625,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="270" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="232" x14ac:dyDescent="0.35">
       <c r="A10" s="18" t="s">
         <v>83</v>
       </c>
@@ -1632,19 +1655,19 @@
       <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="13.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B1" t="str">
         <f>CONDUCTOR_files!E$3</f>
         <v>CONDUCTOR_1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="str">
         <f>B1</f>
         <v>CONDUCTOR_1</v>

</xml_diff>

<commit_message>
chore!: rename variable name in input file
BREAKING CHANGE: renamed variable name VARIABLE_CONTACT_PERIMETER in sheet CONDUCTOR_files of input conductor_definition.xlsx into EXTERNAL_CONTACT_PERIMETER.
This is useful in orther to have a single prefix (EXTERNAL) to distinguish between default (primary or necessary) input files and auxiliary ones.

modified:   input_files/input_file_template/template_conductor_definition.xlsx
</commit_message>
<xml_diff>
--- a/source_code/input_files/input_file_template/template_conductor_definition.xlsx
+++ b/source_code/input_files/input_file_template/template_conductor_definition.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniele.Placido\3D Objects\OPENSC2\source_code\input_files\input_file_template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniele.placido\3D Objects\OPENSC2\source_code\input_files\input_file_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D942AE4-CC28-4E5D-A4BC-B8EB27D3B041}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C80E2BD6-9CA3-43A0-B8EE-5C649020645C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="3330" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CONDUCTOR_files" sheetId="6" r:id="rId1"/>
@@ -302,10 +302,10 @@
     <t xml:space="preserve">current flag: none = current is not defined, bypass the electric module; 0 = constant; -1 = read from file; -2 = external function for current and its derivative after taudum; </t>
   </si>
   <si>
-    <t>VARIABLE_CONTACT_PERIMETER</t>
-  </si>
-  <si>
     <t>external file for variable contact perimeter. Valid extension .xlsx</t>
+  </si>
+  <si>
+    <t>EXTERNAL_CONTACT_PERIMETER</t>
   </si>
 </sst>
 </file>
@@ -459,7 +459,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="TRANSIENT"/>
@@ -789,20 +789,20 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A16" sqref="A16:XFD16"/>
+      <selection pane="bottomRight" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.453125" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.453125" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="33" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.81640625" style="2"/>
+    <col min="6" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>1</v>
       </c>
@@ -815,7 +815,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
       <c r="B2" s="2"/>
       <c r="C2" s="1"/>
@@ -825,7 +825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="str">
         <f>[1]TRANSIENT!A$2</f>
         <v>Variable name</v>
@@ -847,7 +847,7 @@
         <v>CONDUCTOR_1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
@@ -862,7 +862,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>6</v>
       </c>
@@ -877,7 +877,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>7</v>
       </c>
@@ -892,7 +892,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>19</v>
       </c>
@@ -907,7 +907,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>30</v>
       </c>
@@ -922,7 +922,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>13</v>
       </c>
@@ -937,7 +937,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>11</v>
       </c>
@@ -952,7 +952,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>23</v>
       </c>
@@ -967,7 +967,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>20</v>
       </c>
@@ -982,7 +982,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>12</v>
       </c>
@@ -997,7 +997,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>14</v>
       </c>
@@ -1012,7 +1012,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>38</v>
       </c>
@@ -1029,9 +1029,9 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>15</v>
@@ -1040,7 +1040,7 @@
         <v>18</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>61</v>
@@ -1064,17 +1064,17 @@
       <selection pane="bottomRight" activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="2"/>
+    <col min="1" max="1" width="19.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="str">
         <f>CONDUCTOR_files!A$1</f>
         <v>CONDUCTOR</v>
@@ -1088,13 +1088,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E2" s="14">
         <f>IF(E$1 &gt; 0,1,0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="str">
         <f>CONDUCTOR_files!A$3</f>
         <v>Variable name</v>
@@ -1116,7 +1116,7 @@
         <v>CONDUCTOR_1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>78</v>
       </c>
@@ -1133,7 +1133,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>47</v>
       </c>
@@ -1150,7 +1150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>49</v>
       </c>
@@ -1167,7 +1167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>52</v>
       </c>
@@ -1184,7 +1184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>53</v>
       </c>
@@ -1201,7 +1201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>72</v>
       </c>
@@ -1218,7 +1218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>73</v>
       </c>
@@ -1235,7 +1235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>10</v>
       </c>
@@ -1252,7 +1252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>21</v>
       </c>
@@ -1269,7 +1269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>22</v>
       </c>
@@ -1286,7 +1286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>9</v>
       </c>
@@ -1303,7 +1303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>8</v>
       </c>
@@ -1320,7 +1320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>33</v>
       </c>
@@ -1337,7 +1337,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>32</v>
       </c>
@@ -1354,7 +1354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>36</v>
       </c>
@@ -1372,7 +1372,7 @@
         <v>CONDUCTOR_1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" ht="225" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>40</v>
       </c>
@@ -1389,7 +1389,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>43</v>
       </c>
@@ -1406,7 +1406,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>44</v>
       </c>
@@ -1423,7 +1423,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
         <v>74</v>
       </c>
@@ -1440,7 +1440,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
         <v>76</v>
       </c>
@@ -1472,16 +1472,16 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="str">
         <f>CONDUCTOR_files!A1</f>
         <v>CONDUCTOR</v>
@@ -1495,13 +1495,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E2" s="14">
         <f>IF(E$1 &gt;0,1,0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="str">
         <f>CONDUCTOR_files!A$3</f>
         <v>Variable name</v>
@@ -1523,7 +1523,7 @@
         <v>CONDUCTOR_1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="174" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="180" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>62</v>
       </c>
@@ -1540,7 +1540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>64</v>
       </c>
@@ -1557,7 +1557,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="210" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>66</v>
       </c>
@@ -1574,7 +1574,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>69</v>
       </c>
@@ -1591,7 +1591,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="116" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>71</v>
       </c>
@@ -1608,7 +1608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="165" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>80</v>
       </c>
@@ -1625,7 +1625,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="232" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="270" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>83</v>
       </c>
@@ -1655,19 +1655,19 @@
       <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="13.54296875" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" t="str">
         <f>CONDUCTOR_files!E$3</f>
         <v>CONDUCTOR_1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>B1</f>
         <v>CONDUCTOR_1</v>

</xml_diff>

<commit_message>
chore: improve input file fromatting
modified:   input_files/input_file_template/template_conductor_definition.xlsx
</commit_message>
<xml_diff>
--- a/source_code/input_files/input_file_template/template_conductor_definition.xlsx
+++ b/source_code/input_files/input_file_template/template_conductor_definition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniele.placido\3D Objects\OPENSC2\source_code\input_files\input_file_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C80E2BD6-9CA3-43A0-B8EE-5C649020645C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50639E6D-2A5A-43EF-9D6A-FD1B600215A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3330" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4845" yWindow="3855" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CONDUCTOR_files" sheetId="6" r:id="rId1"/>
@@ -785,11 +785,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A17" sqref="A17"/>
+      <selection pane="bottomRight" activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1058,10 +1058,10 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J10" sqref="J10"/>
+      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1458,7 +1458,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1469,7 +1469,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1519,7 +1519,7 @@
         <v>Note/comments</v>
       </c>
       <c r="E3" s="13" t="str">
-        <f>CONDUCTOR_files!E3</f>
+        <f>_xlfn.TEXTJOIN("_",,$A$1,E$1)</f>
         <v>CONDUCTOR_1</v>
       </c>
     </row>
@@ -1651,8 +1651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1662,13 +1662,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B1" t="str">
+      <c r="B1" s="13" t="str">
         <f>CONDUCTOR_files!E$3</f>
         <v>CONDUCTOR_1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="str">
+      <c r="A2" s="13" t="str">
         <f>B1</f>
         <v>CONDUCTOR_1</v>
       </c>
@@ -1678,5 +1678,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat!: new variables in file conductor_definitions.xlsx The new variables are:     *MUTUAL_INDUCTANCE -> Constant value for the mutual inductance used if flag INDUCTANCE_MODE is set to 0.     *SELF_INDUCTANCE -> Constant value used if SELF_INDUCTANCE_MODE is set to 0.
New flag values:
    *INDUCTANCE_MODE = 0 -> constant value from variable MUTUAL_INDUCTANCE
    *SELF_INDUCTANCE_MODE = 0 -> constant value from variable SELF_INDUCTANCE

BREAKING CHANGES
    *New variables MUTUAL_INDUCTANCE, SELF_INDUCTANCE
    *SELF_INDUCTANCE_MODE flag is used whatever is the flag INDUCTANCE_MODE
    *Default value for flag SELF_INDUCTANCE_MODE is changed to 1

modified:   input_files/input_file_template/template_conductor_definition.xlsx
</commit_message>
<xml_diff>
--- a/source_code/input_files/input_file_template/template_conductor_definition.xlsx
+++ b/source_code/input_files/input_file_template/template_conductor_definition.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20406"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniele.placido\3D Objects\OPENSC2\source_code\input_files\input_file_template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\alessandro_mortara\OPENSC2\source_code\input_files\input_file_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C80E2BD6-9CA3-43A0-B8EE-5C649020645C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DB19840-F600-45DC-887E-3147DB2D703B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3330" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="3330" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CONDUCTOR_files" sheetId="6" r:id="rId1"/>
@@ -26,20 +26,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="94">
   <si>
     <t>m</t>
   </si>
@@ -284,12 +276,6 @@
     <t>SELF_INDUCTANCE_MODE</t>
   </si>
   <si>
-    <t>flag to select the method to evaluate the self inductance. Possible values: 1 = mode 1; 2 = mode 2. Used only if flag INDUCTANCE_MODE is set to 1. Defaults to 2</t>
-  </si>
-  <si>
-    <t>flag to select the method to evaluate the inductance. Possible values: 0 = analytical; 1 = approximated. Defaults to 1.</t>
-  </si>
-  <si>
     <t>ELECTRIC_SOLVER</t>
   </si>
   <si>
@@ -306,6 +292,27 @@
   </si>
   <si>
     <t>EXTERNAL_CONTACT_PERIMETER</t>
+  </si>
+  <si>
+    <t>MUTUAL_INDUCTANCE</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>SELF_INDUCTANCE</t>
+  </si>
+  <si>
+    <t>flag to select the method to evaluate the inductance. Possible values: 0 = constant value from variable MUTUAL_INDUCTANCE; 1 = analytical; 2 = approximated. Defaults to 1.</t>
+  </si>
+  <si>
+    <t>Constant value for the mutual inductance used if flag INDUCTANCE_MODE is set to 0.</t>
+  </si>
+  <si>
+    <t>flag to select the method to evaluate the self inductance. Possible values: 0 = constant value from variable SEL_INDUCTANCE; 1 = mode 1; 2 = mode 2. Defaults to 1</t>
+  </si>
+  <si>
+    <t>Constant value used if SELF_INDUCTANCE_MODE is set to 0.</t>
   </si>
 </sst>
 </file>
@@ -361,7 +368,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -440,6 +447,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -785,7 +795,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
@@ -1031,7 +1041,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>15</v>
@@ -1040,7 +1050,7 @@
         <v>18</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>61</v>
@@ -1212,7 +1222,7 @@
         <v>17</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E9" s="5">
         <v>0</v>
@@ -1451,7 +1461,7 @@
         <v>16</v>
       </c>
       <c r="D23" s="22" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E23" s="19" t="s">
         <v>77</v>
@@ -1466,10 +1476,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC5BD13E-E4E6-4E9C-8F28-77E32E58E378}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1591,7 +1601,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>71</v>
       </c>
@@ -1602,32 +1612,32 @@
         <v>17</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="E8" s="17">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="E9" s="23">
+        <v>4.9999999999999998E-8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="134.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="18" t="s">
         <v>80</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="E9" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="270" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
-        <v>83</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>15</v>
@@ -1636,9 +1646,43 @@
         <v>17</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="E10" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="E11" s="23">
+        <v>9.9999999999999995E-8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="270" x14ac:dyDescent="0.25">
+      <c r="A12" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="E12" s="17">
         <v>1</v>
       </c>
     </row>

</xml_diff>